<commit_message>
show a base ui
</commit_message>
<xml_diff>
--- a/问题记录.xlsx
+++ b/问题记录.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>imgui环境配置问题：</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>然后再配置lib库，这个imgui.lib记得配置，之前就是因为这个没配置，所以环境一直报错</t>
+  </si>
+  <si>
+    <t>关于在使用imgui的时候，ui</t>
+  </si>
+  <si>
+    <t>是渲染顺序出错了，图片中标蓝的这一段代码，应该放在加载imgui这一段代码后面，</t>
+  </si>
+  <si>
+    <t>一直显示不出来的问题</t>
+  </si>
+  <si>
+    <t>具体原因我个人猜测是因为设置了深度测试后，ui的深度值比较小，所以会被背景给覆盖掉。</t>
+  </si>
+  <si>
+    <t>所以把深度测试在ui加载好了后在开启，就不会把ui挡住了。</t>
   </si>
 </sst>
 </file>
@@ -792,6 +807,48 @@
         <a:xfrm>
           <a:off x="1805940" y="2971800"/>
           <a:ext cx="5637530" cy="2868930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5654675</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>163195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1805940" y="5852160"/>
+          <a:ext cx="5654675" cy="5100955"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1057,10 +1114,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1082,6 +1139,27 @@
     <row r="17" spans="3:3">
       <c r="C17" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add simple ui class 70%
</commit_message>
<xml_diff>
--- a/问题记录.xlsx
+++ b/问题记录.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>imgui环境配置问题：</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>具体为什么只能在main中添加宏定义，暂时还不知道原因。</t>
+  </si>
+  <si>
+    <t>在配置环境的时候，最好把依</t>
+  </si>
+  <si>
+    <t>最好给文件专门建个文件夹，把依赖的库的代码都放在里面，然后用的时候就能直接用了，不用再去索引。</t>
+  </si>
+  <si>
+    <t>赖库都放在代码里面</t>
+  </si>
+  <si>
+    <t>左边这个就是因为没有放到文件里，是额外链接的，然后再手动点了“包括在项目内”。这样还是会麻烦点的。</t>
   </si>
 </sst>
 </file>
@@ -1062,6 +1074,48 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5000625</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="图片 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1805940" y="18470880"/>
+          <a:ext cx="5000625" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1315,10 +1369,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1395,6 +1449,22 @@
     <row r="93" spans="3:3">
       <c r="C93" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>